<commit_message>
updates new scripts and results during revision
</commit_message>
<xml_diff>
--- a/00_DATA/actual_sampling.xlsx
+++ b/00_DATA/actual_sampling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/rb979_cam_ac_uk/Documents/Desktop/COVID-19_Vaccination_GM/00_DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebecca/Library/CloudStorage/OneDrive-UniversityofCambridge/Desktop/COVID-19_Vaccination_GM/00_DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{67414822-62B3-AD44-BD7C-8ADF4B89C7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DE45A37-D20F-CF4B-9CC9-F424DF43A475}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91C9270-E05E-C644-8ED4-6BE41D8602B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-480" windowWidth="38400" windowHeight="21100" xr2:uid="{45BE0998-7C02-5648-A5BE-370E1A6FABC1}"/>
+    <workbookView xWindow="-24960" yWindow="-480" windowWidth="38400" windowHeight="21100" xr2:uid="{45BE0998-7C02-5648-A5BE-370E1A6FABC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -314,11 +314,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -331,6 +390,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,10 +421,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -652,55 +722,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253EAA58-4152-E54D-A582-C31954B06931}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="10.83203125" style="1"/>
+    <col min="1" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="7" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.83203125" style="5"/>
+    <col min="10" max="11" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1">
@@ -712,7 +786,7 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>1</v>
       </c>
       <c r="G2" s="1">
@@ -721,7 +795,7 @@
       <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="5">
         <v>0</v>
       </c>
       <c r="J2" s="1">
@@ -747,7 +821,7 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
       <c r="G3" s="1">
@@ -756,7 +830,7 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="5">
         <v>0</v>
       </c>
       <c r="J3" s="1">
@@ -782,7 +856,7 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>0</v>
       </c>
       <c r="G4" s="1">
@@ -791,7 +865,7 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="5">
         <v>1</v>
       </c>
       <c r="J4" s="1">
@@ -817,7 +891,7 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>0</v>
       </c>
       <c r="G5" s="1">
@@ -826,14 +900,14 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="5">
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -852,20 +926,20 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="5">
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -887,7 +961,7 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="1">
@@ -896,7 +970,7 @@
       <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="5">
         <v>1</v>
       </c>
       <c r="J7" s="1">
@@ -922,7 +996,7 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="5">
         <v>0</v>
       </c>
       <c r="G8" s="1">
@@ -931,7 +1005,7 @@
       <c r="H8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="5">
         <v>1</v>
       </c>
       <c r="J8" s="1">
@@ -957,7 +1031,7 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="5">
         <v>0</v>
       </c>
       <c r="G9" s="1">
@@ -966,7 +1040,7 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="5">
         <v>1</v>
       </c>
       <c r="J9" s="1">
@@ -992,7 +1066,7 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="5">
         <v>0</v>
       </c>
       <c r="G10" s="1">
@@ -1001,7 +1075,7 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="5">
         <v>0</v>
       </c>
       <c r="J10" s="1">
@@ -1027,7 +1101,7 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="5">
         <v>0</v>
       </c>
       <c r="G11" s="1">
@@ -1036,7 +1110,7 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="5">
         <v>1</v>
       </c>
       <c r="J11" s="1">
@@ -1062,7 +1136,7 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="5">
         <v>0</v>
       </c>
       <c r="G12" s="1">
@@ -1071,7 +1145,7 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="5">
         <v>0</v>
       </c>
       <c r="J12" s="1">
@@ -1097,7 +1171,7 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="5">
         <v>0</v>
       </c>
       <c r="G13" s="1">
@@ -1106,7 +1180,7 @@
       <c r="H13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="5">
         <v>1</v>
       </c>
       <c r="J13" s="1">
@@ -1132,7 +1206,7 @@
       <c r="E14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="5">
         <v>0</v>
       </c>
       <c r="G14" s="1">
@@ -1141,7 +1215,7 @@
       <c r="H14" s="1">
         <v>0</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="5">
         <v>1</v>
       </c>
       <c r="J14" s="1">
@@ -1167,7 +1241,7 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="5">
         <v>0</v>
       </c>
       <c r="G15" s="1">
@@ -1176,7 +1250,7 @@
       <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="5">
         <v>1</v>
       </c>
       <c r="J15" s="1">
@@ -1202,7 +1276,7 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="5">
         <v>0</v>
       </c>
       <c r="G16" s="1">
@@ -1211,7 +1285,7 @@
       <c r="H16" s="1">
         <v>0</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="5">
         <v>1</v>
       </c>
       <c r="J16" s="1">
@@ -1237,7 +1311,7 @@
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="5">
         <v>0</v>
       </c>
       <c r="G17" s="1">
@@ -1246,7 +1320,7 @@
       <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="5">
         <v>1</v>
       </c>
       <c r="J17" s="1">
@@ -1272,7 +1346,7 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="5">
         <v>0</v>
       </c>
       <c r="G18" s="1">
@@ -1281,7 +1355,7 @@
       <c r="H18" s="1">
         <v>1</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="5">
         <v>1</v>
       </c>
       <c r="J18" s="1">
@@ -1307,7 +1381,7 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="5">
         <v>0</v>
       </c>
       <c r="G19" s="1">
@@ -1316,7 +1390,7 @@
       <c r="H19" s="1">
         <v>1</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="5">
         <v>0</v>
       </c>
       <c r="J19" s="1">
@@ -1342,7 +1416,7 @@
       <c r="E20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="5">
         <v>0</v>
       </c>
       <c r="G20" s="1">
@@ -1351,7 +1425,7 @@
       <c r="H20" s="1">
         <v>1</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="5">
         <v>1</v>
       </c>
       <c r="J20" s="1">
@@ -1369,7 +1443,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1377,7 +1451,7 @@
       <c r="E21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="5">
         <v>0</v>
       </c>
       <c r="G21" s="1">
@@ -1386,8 +1460,8 @@
       <c r="H21" s="1">
         <v>1</v>
       </c>
-      <c r="I21" s="1">
-        <v>1</v>
+      <c r="I21" s="5">
+        <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
@@ -1412,7 +1486,7 @@
       <c r="E22" s="1">
         <v>1</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="5">
         <v>0</v>
       </c>
       <c r="G22" s="1">
@@ -1421,7 +1495,7 @@
       <c r="H22" s="1">
         <v>1</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="5">
         <v>0</v>
       </c>
       <c r="J22" s="1">
@@ -1447,7 +1521,7 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="5">
         <v>0</v>
       </c>
       <c r="G23" s="1">
@@ -1456,7 +1530,7 @@
       <c r="H23" s="1">
         <v>1</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="5">
         <v>1</v>
       </c>
       <c r="J23" s="1">
@@ -1482,7 +1556,7 @@
       <c r="E24" s="1">
         <v>1</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="5">
         <v>0</v>
       </c>
       <c r="G24" s="1">
@@ -1491,7 +1565,7 @@
       <c r="H24" s="1">
         <v>1</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="5">
         <v>1</v>
       </c>
       <c r="J24" s="1">
@@ -1517,7 +1591,7 @@
       <c r="E25" s="1">
         <v>0</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="5">
         <v>0</v>
       </c>
       <c r="G25" s="1">
@@ -1526,7 +1600,7 @@
       <c r="H25" s="1">
         <v>1</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="5">
         <v>0</v>
       </c>
       <c r="J25" s="1">
@@ -1552,7 +1626,7 @@
       <c r="E26" s="1">
         <v>0</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="5">
         <v>0</v>
       </c>
       <c r="G26" s="1">
@@ -1561,7 +1635,7 @@
       <c r="H26" s="1">
         <v>1</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="5">
         <v>0</v>
       </c>
       <c r="J26" s="1">
@@ -1587,7 +1661,7 @@
       <c r="E27" s="1">
         <v>0</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="5">
         <v>0</v>
       </c>
       <c r="G27" s="1">
@@ -1596,7 +1670,7 @@
       <c r="H27" s="1">
         <v>1</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="5">
         <v>0</v>
       </c>
       <c r="J27" s="1">
@@ -1622,7 +1696,7 @@
       <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="5">
         <v>0</v>
       </c>
       <c r="G28" s="1">
@@ -1631,7 +1705,7 @@
       <c r="H28" s="1">
         <v>1</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="5">
         <v>1</v>
       </c>
       <c r="J28" s="1">
@@ -1657,7 +1731,7 @@
       <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="5">
         <v>0</v>
       </c>
       <c r="G29" s="1">
@@ -1666,7 +1740,7 @@
       <c r="H29" s="1">
         <v>1</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="5">
         <v>0</v>
       </c>
       <c r="J29" s="1">
@@ -1692,7 +1766,7 @@
       <c r="E30" s="1">
         <v>1</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="5">
         <v>0</v>
       </c>
       <c r="G30" s="1">
@@ -1701,7 +1775,7 @@
       <c r="H30" s="1">
         <v>1</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="5">
         <v>1</v>
       </c>
       <c r="J30" s="1">
@@ -1727,7 +1801,7 @@
       <c r="E31" s="1">
         <v>1</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="5">
         <v>0</v>
       </c>
       <c r="G31" s="1">
@@ -1736,7 +1810,7 @@
       <c r="H31" s="1">
         <v>1</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31" s="5">
         <v>0</v>
       </c>
       <c r="J31" s="1">
@@ -1754,15 +1828,15 @@
         <v>30</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="5">
         <v>0</v>
       </c>
       <c r="G32" s="1">
@@ -1771,7 +1845,7 @@
       <c r="H32" s="1">
         <v>1</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32" s="5">
         <v>0</v>
       </c>
       <c r="J32" s="1">
@@ -1797,7 +1871,7 @@
       <c r="E33" s="1">
         <v>0</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="5">
         <v>0</v>
       </c>
       <c r="G33" s="1">
@@ -1806,7 +1880,7 @@
       <c r="H33" s="1">
         <v>1</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33" s="5">
         <v>1</v>
       </c>
       <c r="J33" s="1">
@@ -1832,16 +1906,16 @@
       <c r="E34" s="1">
         <v>0</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="5">
         <v>0</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
       </c>
       <c r="H34" s="1">
-        <v>1</v>
-      </c>
-      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
         <v>0</v>
       </c>
       <c r="J34" s="1">
@@ -1867,7 +1941,7 @@
       <c r="E35" s="1">
         <v>0</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="5">
         <v>0</v>
       </c>
       <c r="G35" s="1">
@@ -1876,7 +1950,7 @@
       <c r="H35" s="1">
         <v>0</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="5">
         <v>0</v>
       </c>
       <c r="J35" s="1">
@@ -1902,7 +1976,7 @@
       <c r="E36" s="1">
         <v>0</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="5">
         <v>0</v>
       </c>
       <c r="G36" s="1">
@@ -1911,7 +1985,7 @@
       <c r="H36" s="1">
         <v>1</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="5">
         <v>1</v>
       </c>
       <c r="J36" s="1">
@@ -1937,7 +2011,7 @@
       <c r="E37" s="1">
         <v>0</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="5">
         <v>0</v>
       </c>
       <c r="G37" s="1">
@@ -1946,7 +2020,7 @@
       <c r="H37" s="1">
         <v>1</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="5">
         <v>1</v>
       </c>
       <c r="J37" s="1">
@@ -1972,7 +2046,7 @@
       <c r="E38" s="1">
         <v>0</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="5">
         <v>0</v>
       </c>
       <c r="G38" s="1">
@@ -1981,7 +2055,7 @@
       <c r="H38" s="1">
         <v>1</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="5">
         <v>1</v>
       </c>
       <c r="J38" s="1">
@@ -2007,7 +2081,7 @@
       <c r="E39" s="1">
         <v>0</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="5">
         <v>0</v>
       </c>
       <c r="G39" s="1">
@@ -2016,7 +2090,7 @@
       <c r="H39" s="1">
         <v>1</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="5">
         <v>1</v>
       </c>
       <c r="J39" s="1">
@@ -2042,7 +2116,7 @@
       <c r="E40" s="1">
         <v>0</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="5">
         <v>0</v>
       </c>
       <c r="G40" s="1">
@@ -2051,7 +2125,7 @@
       <c r="H40" s="1">
         <v>1</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="5">
         <v>1</v>
       </c>
       <c r="J40" s="1">
@@ -2077,7 +2151,7 @@
       <c r="E41" s="1">
         <v>0</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="5">
         <v>0</v>
       </c>
       <c r="G41" s="1">
@@ -2086,7 +2160,7 @@
       <c r="H41" s="1">
         <v>1</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="5">
         <v>0</v>
       </c>
       <c r="J41" s="1">
@@ -2112,7 +2186,7 @@
       <c r="E42" s="1">
         <v>0</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="5">
         <v>0</v>
       </c>
       <c r="G42" s="1">
@@ -2121,7 +2195,7 @@
       <c r="H42" s="1">
         <v>1</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42" s="5">
         <v>1</v>
       </c>
       <c r="J42" s="1">
@@ -2147,7 +2221,7 @@
       <c r="E43" s="1">
         <v>0</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="5">
         <v>0</v>
       </c>
       <c r="G43" s="1">
@@ -2156,7 +2230,7 @@
       <c r="H43" s="1">
         <v>1</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43" s="5">
         <v>1</v>
       </c>
       <c r="J43" s="1">
@@ -2182,7 +2256,7 @@
       <c r="E44" s="1">
         <v>0</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="5">
         <v>0</v>
       </c>
       <c r="G44" s="1">
@@ -2191,7 +2265,7 @@
       <c r="H44" s="1">
         <v>1</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44" s="5">
         <v>1</v>
       </c>
       <c r="J44" s="1">
@@ -2217,7 +2291,7 @@
       <c r="E45" s="1">
         <v>0</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="5">
         <v>0</v>
       </c>
       <c r="G45" s="1">
@@ -2226,7 +2300,7 @@
       <c r="H45" s="1">
         <v>1</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I45" s="5">
         <v>1</v>
       </c>
       <c r="J45" s="1">
@@ -2252,7 +2326,7 @@
       <c r="E46" s="1">
         <v>0</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="5">
         <v>0</v>
       </c>
       <c r="G46" s="1">
@@ -2261,7 +2335,7 @@
       <c r="H46" s="1">
         <v>1</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46" s="5">
         <v>1</v>
       </c>
       <c r="J46" s="1">
@@ -2287,7 +2361,7 @@
       <c r="E47" s="1">
         <v>1</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="5">
         <v>0</v>
       </c>
       <c r="G47" s="1">
@@ -2296,7 +2370,7 @@
       <c r="H47" s="1">
         <v>1</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47" s="5">
         <v>0</v>
       </c>
       <c r="J47" s="1">
@@ -2322,7 +2396,7 @@
       <c r="E48" s="1">
         <v>0</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="5">
         <v>0</v>
       </c>
       <c r="G48" s="1">
@@ -2331,7 +2405,7 @@
       <c r="H48" s="1">
         <v>0</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48" s="5">
         <v>1</v>
       </c>
       <c r="J48" s="1">
@@ -2357,7 +2431,7 @@
       <c r="E49" s="1">
         <v>0</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="5">
         <v>0</v>
       </c>
       <c r="G49" s="1">
@@ -2366,7 +2440,7 @@
       <c r="H49" s="1">
         <v>0</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49" s="5">
         <v>1</v>
       </c>
       <c r="J49" s="1">
@@ -2392,7 +2466,7 @@
       <c r="E50" s="1">
         <v>0</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="5">
         <v>0</v>
       </c>
       <c r="G50" s="1">
@@ -2401,7 +2475,7 @@
       <c r="H50" s="1">
         <v>0</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50" s="5">
         <v>1</v>
       </c>
       <c r="J50" s="1">
@@ -2427,7 +2501,7 @@
       <c r="E51" s="1">
         <v>0</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="5">
         <v>0</v>
       </c>
       <c r="G51" s="1">
@@ -2436,7 +2510,7 @@
       <c r="H51" s="1">
         <v>0</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51" s="5">
         <v>0</v>
       </c>
       <c r="J51" s="1">
@@ -2462,7 +2536,7 @@
       <c r="E52" s="1">
         <v>1</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="5">
         <v>0</v>
       </c>
       <c r="G52" s="1">
@@ -2471,7 +2545,7 @@
       <c r="H52" s="1">
         <v>1</v>
       </c>
-      <c r="I52" s="1">
+      <c r="I52" s="5">
         <v>0</v>
       </c>
       <c r="J52" s="1">
@@ -2497,7 +2571,7 @@
       <c r="E53" s="1">
         <v>1</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53" s="5">
         <v>0</v>
       </c>
       <c r="G53" s="1">
@@ -2506,7 +2580,7 @@
       <c r="H53" s="1">
         <v>1</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I53" s="5">
         <v>0</v>
       </c>
       <c r="J53" s="1">
@@ -2532,7 +2606,7 @@
       <c r="E54" s="1">
         <v>0</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F54" s="5">
         <v>0</v>
       </c>
       <c r="G54" s="1">
@@ -2541,7 +2615,7 @@
       <c r="H54" s="1">
         <v>1</v>
       </c>
-      <c r="I54" s="1">
+      <c r="I54" s="5">
         <v>0</v>
       </c>
       <c r="J54" s="1">
@@ -2567,7 +2641,7 @@
       <c r="E55" s="1">
         <v>1</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="5">
         <v>0</v>
       </c>
       <c r="G55" s="1">
@@ -2576,7 +2650,7 @@
       <c r="H55" s="1">
         <v>1</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I55" s="5">
         <v>0</v>
       </c>
       <c r="J55" s="1">
@@ -2602,7 +2676,7 @@
       <c r="E56" s="1">
         <v>1</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56" s="5">
         <v>0</v>
       </c>
       <c r="G56" s="1">
@@ -2611,7 +2685,7 @@
       <c r="H56" s="1">
         <v>1</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I56" s="5">
         <v>0</v>
       </c>
       <c r="J56" s="1">
@@ -2637,7 +2711,7 @@
       <c r="E57" s="1">
         <v>1</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57" s="5">
         <v>0</v>
       </c>
       <c r="G57" s="1">
@@ -2646,7 +2720,7 @@
       <c r="H57" s="1">
         <v>1</v>
       </c>
-      <c r="I57" s="1">
+      <c r="I57" s="5">
         <v>0</v>
       </c>
       <c r="J57" s="1">
@@ -2672,7 +2746,7 @@
       <c r="E58" s="1">
         <v>0</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F58" s="5">
         <v>0</v>
       </c>
       <c r="G58" s="1">
@@ -2681,7 +2755,7 @@
       <c r="H58" s="1">
         <v>1</v>
       </c>
-      <c r="I58" s="1">
+      <c r="I58" s="5">
         <v>1</v>
       </c>
       <c r="J58" s="1">
@@ -2707,7 +2781,7 @@
       <c r="E59" s="1">
         <v>0</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="5">
         <v>1</v>
       </c>
       <c r="G59" s="1">
@@ -2716,7 +2790,7 @@
       <c r="H59" s="1">
         <v>1</v>
       </c>
-      <c r="I59" s="1">
+      <c r="I59" s="5">
         <v>0</v>
       </c>
       <c r="J59" s="1">
@@ -2742,16 +2816,16 @@
       <c r="E60" s="1">
         <v>0</v>
       </c>
-      <c r="F60" s="1">
-        <v>0</v>
+      <c r="F60" s="5">
+        <v>1</v>
       </c>
       <c r="G60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" s="1">
         <v>1</v>
       </c>
-      <c r="I60" s="1">
+      <c r="I60" s="5">
         <v>0</v>
       </c>
       <c r="J60" s="1">

</xml_diff>